<commit_message>
Fixed validation of fields.
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>Oskar</t>
   </si>
@@ -132,6 +132,18 @@
     <t>200101</t>
   </si>
   <si>
+    <t>19930718-1111</t>
+  </si>
+  <si>
+    <t>SE0000106270</t>
+  </si>
+  <si>
+    <t>2018-11-02</t>
+  </si>
+  <si>
+    <t>200,2</t>
+  </si>
+  <si>
     <t>Registered at</t>
   </si>
   <si>
@@ -169,9 +181,6 @@
   </si>
   <si>
     <t>150</t>
-  </si>
-  <si>
-    <t>19930718-1111</t>
   </si>
   <si>
     <t>SE1233435000</t>
@@ -232,7 +241,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -488,6 +497,38 @@
       </c>
       <c r="J9">
         <v>40000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43413.53868383102</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10">
+        <v>40040</v>
       </c>
     </row>
   </sheetData>
@@ -502,34 +543,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -540,13 +581,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
         <v>22</v>
@@ -555,7 +596,7 @@
         <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
@@ -577,34 +618,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -615,13 +656,13 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
         <v>22</v>

</xml_diff>